<commit_message>
Add unit tests and convergence estimation
</commit_message>
<xml_diff>
--- a/probability/result.xlsx
+++ b/probability/result.xlsx
@@ -19,19 +19,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>n</t>
   </si>
   <si>
     <t>p</t>
   </si>
+  <si>
+    <t>ln(n)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Δp = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|p_практ - p_теор|</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ln(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Δp)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +227,13 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="33">
@@ -366,7 +417,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -540,6 +591,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -585,13 +675,22 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -637,13 +736,51 @@
     <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="26">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -745,6 +882,13 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -752,21 +896,12 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -784,12 +919,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
+        <top/>
+        <bottom/>
+        <vertical style="thin">
           <color indexed="64"/>
-        </top>
-        <bottom style="thin">
+        </vertical>
+        <horizontal style="thin">
           <color indexed="64"/>
-        </bottom>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -822,6 +959,36 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -840,10 +1007,55 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -861,12 +1073,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
+        <top/>
+        <bottom/>
+        <vertical style="thin">
           <color indexed="64"/>
-        </top>
-        <bottom style="thin">
+        </vertical>
+        <horizontal style="thin">
           <color indexed="64"/>
-        </bottom>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -943,7 +1157,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1689,7 +1902,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1809,7 +2021,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4015,6 +4226,529 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Оценка</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> сходимости</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="ru-RU"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>result!$AF$2:$AF$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.3862943611198906</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8501476017100584</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.1612073216950769</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4536142097733666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.770735088230952</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.060783674643254</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.201137696540702</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>result!$AH$2:$AH$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-1.4863799249422471</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.5639368701997971</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5.62238683645222</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.9485059226307007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-7.6777835038780591</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-9.293721980915441</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-8.1387567556961322</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E5EE-4F2E-B8BD-A8C66EFF110F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="333393464"/>
+        <c:axId val="333395104"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="333393464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="16"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ln(n)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333395104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="333395104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="-1"/>
+          <c:min val="-10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ln(</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR"/>
+                  <a:t>Δ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>p)</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="333393464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4135,6 +4869,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5168,6 +5942,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5781,37 +7071,86 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Диаграмма 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:B101" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:B101" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="A1:B101"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="n" dataDxfId="13"/>
-    <tableColumn id="2" name="p" dataDxfId="12"/>
+    <tableColumn id="1" name="n" dataDxfId="21"/>
+    <tableColumn id="2" name="p" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="K1:L101" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Таблица2" displayName="Таблица2" ref="K1:L101" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="K1:L101"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="n" dataDxfId="7"/>
-    <tableColumn id="2" name="p" dataDxfId="6"/>
+    <tableColumn id="1" name="n" dataDxfId="15"/>
+    <tableColumn id="2" name="p" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="U1:V101" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Таблица3" displayName="Таблица3" ref="U1:V101" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="U1:V101"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="n" dataDxfId="1"/>
-    <tableColumn id="2" name="p" dataDxfId="0"/>
+    <tableColumn id="1" name="n" dataDxfId="9"/>
+    <tableColumn id="2" name="p" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Таблица4" displayName="Таблица4" ref="AE1:AH8" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="AE1:AH8"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="n" dataDxfId="3"/>
+    <tableColumn id="2" name="ln(n)" dataDxfId="1">
+      <calculatedColumnFormula xml:space="preserve"> LN(Таблица4[[#This Row],[n]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Δp = |p_практ - p_теор|" dataDxfId="2"/>
+    <tableColumn id="4" name="ln(Δp)" dataDxfId="0">
+      <calculatedColumnFormula xml:space="preserve"> LN(Таблица4[[#This Row],[Δp = |p_практ - p_теор|]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6080,10 +7419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V101"/>
+  <dimension ref="A1:AR101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AD20" sqref="AD20"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AS14" sqref="AS14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6094,9 +7433,13 @@
     <col min="12" max="12" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6115,8 +7458,20 @@
       <c r="V1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="AE1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <f xml:space="preserve"> 1</f>
         <v>1</v>
@@ -6136,8 +7491,23 @@
       <c r="V2" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="AE2" s="3">
+        <v>4</v>
+      </c>
+      <c r="AF2" s="4">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[n]])</f>
+        <v>1.3862943611198906</v>
+      </c>
+      <c r="AG2" s="8">
+        <f xml:space="preserve"> ABS(0.75 - 0.52381)</f>
+        <v>0.22619</v>
+      </c>
+      <c r="AH2" s="6">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[Δp = |p_практ - p_теор|]])</f>
+        <v>-1.4863799249422471</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <f xml:space="preserve"> A2 + 1</f>
         <v>2</v>
@@ -6159,8 +7529,23 @@
       <c r="V3" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="AE3" s="3">
+        <v>47</v>
+      </c>
+      <c r="AF3" s="9">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[n]])</f>
+        <v>3.8501476017100584</v>
+      </c>
+      <c r="AG3" s="10">
+        <f xml:space="preserve"> ABS(0.446809 - 0.52381)</f>
+        <v>7.7000999999999986E-2</v>
+      </c>
+      <c r="AH3" s="6">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[Δp = |p_практ - p_теор|]])</f>
+        <v>-2.5639368701997971</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A67" si="0" xml:space="preserve"> A3 + 1</f>
         <v>3</v>
@@ -6182,8 +7567,23 @@
       <c r="V4" s="4">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="AE4" s="3">
+        <v>474</v>
+      </c>
+      <c r="AF4" s="9">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[n]])</f>
+        <v>6.1612073216950769</v>
+      </c>
+      <c r="AG4" s="10">
+        <f xml:space="preserve"> 0.527426 - 0.52381</f>
+        <v>3.6159999999999526E-3</v>
+      </c>
+      <c r="AH4" s="6">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[Δp = |p_практ - p_теор|]])</f>
+        <v>-5.62238683645222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6205,8 +7605,23 @@
       <c r="V5" s="4">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="AE5" s="3">
+        <v>4692</v>
+      </c>
+      <c r="AF5" s="9">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[n]])</f>
+        <v>8.4536142097733666</v>
+      </c>
+      <c r="AG5" s="10">
+        <f xml:space="preserve"> 0.530904 - 0.52381</f>
+        <v>7.0940000000000447E-3</v>
+      </c>
+      <c r="AH5" s="6">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[Δp = |p_практ - p_теор|]])</f>
+        <v>-4.9485059226307007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6228,8 +7643,23 @@
       <c r="V6" s="4">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="AE6" s="3">
+        <v>47607</v>
+      </c>
+      <c r="AF6" s="9">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[n]])</f>
+        <v>10.770735088230952</v>
+      </c>
+      <c r="AG6" s="10">
+        <f xml:space="preserve"> ABS(0.523347 - 0.52381)</f>
+        <v>4.629999999999912E-4</v>
+      </c>
+      <c r="AH6" s="6">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[Δp = |p_практ - p_теор|]])</f>
+        <v>-7.6777835038780591</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6251,8 +7681,23 @@
       <c r="V7" s="4">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="AE7" s="3">
+        <v>470139</v>
+      </c>
+      <c r="AF7" s="9">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[n]])</f>
+        <v>13.060783674643254</v>
+      </c>
+      <c r="AG7" s="10">
+        <f xml:space="preserve"> 0.523902 - 0.52381</f>
+        <v>9.1999999999980986E-5</v>
+      </c>
+      <c r="AH7" s="6">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[Δp = |p_практ - p_теор|]])</f>
+        <v>-9.293721980915441</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6274,8 +7719,23 @@
       <c r="V8" s="4">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="AE8" s="6">
+        <v>3997332</v>
+      </c>
+      <c r="AF8" s="9">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[n]])</f>
+        <v>15.201137696540702</v>
+      </c>
+      <c r="AG8" s="8">
+        <f xml:space="preserve"> ABS(0.523518 - 0.52381)</f>
+        <v>2.9199999999995896E-4</v>
+      </c>
+      <c r="AH8" s="6">
+        <f xml:space="preserve"> LN(Таблица4[[#This Row],[Δp = |p_практ - p_теор|]])</f>
+        <v>-8.1387567556961322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6297,8 +7757,11 @@
       <c r="V9" s="4">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="12"/>
+      <c r="AG9" s="13"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6321,7 +7784,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6344,7 +7807,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6367,7 +7830,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -6390,7 +7853,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -6413,7 +7876,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -6436,7 +7899,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8416,11 +9879,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <tableParts count="3">
-    <tablePart r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="4">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>